<commit_message>
Added more linked coverage to U-mode vplan
Signed-off-by: Henrik Fegran <Henrik.Fegran@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/privileged_spec/CV32E40S_UserMode.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/privileged_spec/CV32E40S_UserMode.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\openhw\core-v-verif_40s\cv32e40s\docs\VerifPlans\Simulation\privileged_spec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hefegran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A65AE6-7AAF-4D93-A713-4748CF5D3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DA8124-A142-354F-94F0-97B14208EDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-level Feature" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="298">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -1074,17 +1074,10 @@
     <t>JVT is the only URW CSR. Write and nread operations in User mode must be covered</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>A:a_dt_instr_trigger_hit_*, a_dt_load_trigger_hit_*, a_dt_store_trigger_hit_*, a_dt_exception_trigger_hit_*, a_dt_enter_dbg_reason, a_dt_tie_offs_*</t>
   </si>
   <si>
     <t xml:space="preserve">A: a_dt_exception_trigger_hit_*, a_dt_enter_dbg_reason, a_dt_warl_tselect, a_dt_warl_tdata1_general, a_dt_warl_tdata1_m2, a_dt_warl_tdata1_etrigger, a_dt_warl_tdata1_m6, a_dt_warl_tdata1_disabled, a_dt_warl_tdata2_etrigger, a_dt_warl_tinfo. </t>
-  </si>
-  <si>
-    <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.umode_assert_i.a_jvt_access
-COV: TODO</t>
   </si>
   <si>
     <t>A: a_dt_no_access_to_tdata_in_umode
@@ -1093,6 +1086,18 @@
   <si>
     <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.core_i.clic_assert_i.gen_clic_assertions.a_mret_pc_intended,
 A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.core_i.clic_assert_i.gen_clic_assertions.a_dret_pc_intended,</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.umode_assert_i.a_jvt_access
+DTC: cv32e40s/tests/programs/custom/zcmt_test</t>
+  </si>
+  <si>
+    <t>DTC: cv32e40s/tests/programs/custom/zcmt_test :: jvt_rw_m, jvt_rw_u_illegal, jvt_rw_u_legal</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.clic_assert_i.a_mscratchcsw_value
+COV: ???
+DTC: cv32e40s/tests/programs/custom/clic :: rw_mscratchcsw, rw_mscratchcsw_illegal</t>
   </si>
 </sst>
 </file>
@@ -1174,6 +1179,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1243,13 +1249,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1636,28 +1642,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" customWidth="1"/>
     <col min="9" max="9" width="120" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" customWidth="1"/>
-    <col min="1024" max="1024" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="30.5" customWidth="1"/>
+    <col min="1024" max="1024" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="30">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="32">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1689,7 +1695,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="115.15" customHeight="1">
+    <row r="2" spans="1:10" ht="115.25" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>33</v>
       </c>
@@ -1719,7 +1725,7 @@
       </c>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:10" ht="47.45" customHeight="1">
+    <row r="3" spans="1:10" ht="47.5" customHeight="1">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
@@ -1799,7 +1805,7 @@
       </c>
       <c r="J5" s="13"/>
     </row>
-    <row r="6" spans="1:10" ht="99.75">
+    <row r="6" spans="1:10" ht="112">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
@@ -1851,7 +1857,7 @@
       </c>
       <c r="J7" s="13"/>
     </row>
-    <row r="8" spans="1:10" ht="178.9" customHeight="1">
+    <row r="8" spans="1:10" ht="179" customHeight="1">
       <c r="A8" s="13" t="s">
         <v>33</v>
       </c>
@@ -1881,7 +1887,7 @@
       </c>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10" ht="156.6" customHeight="1">
+    <row r="9" spans="1:10" ht="156.5" customHeight="1">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
@@ -1929,7 +1935,7 @@
         <v>15</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="J10" s="13"/>
     </row>
@@ -1985,7 +1991,7 @@
       </c>
       <c r="J12" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="171">
+    <row r="13" spans="1:10" ht="208">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13" t="s">
@@ -2037,7 +2043,7 @@
       </c>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" spans="1:10" ht="91.9" customHeight="1">
+    <row r="15" spans="1:10" ht="92" customHeight="1">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
@@ -2059,7 +2065,7 @@
         <v>24</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>231</v>
+        <v>297</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>261</v>
@@ -2091,7 +2097,7 @@
       </c>
       <c r="J16" s="13"/>
     </row>
-    <row r="17" spans="1:10" ht="28.5">
+    <row r="17" spans="1:10" ht="32">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13" t="s">
@@ -2117,7 +2123,7 @@
       </c>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" spans="1:10" ht="167.45" customHeight="1">
+    <row r="18" spans="1:10" ht="167.5" customHeight="1">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
@@ -2143,7 +2149,7 @@
       </c>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="1:10" ht="57">
+    <row r="19" spans="1:10" ht="80">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13" t="s">
@@ -2169,7 +2175,7 @@
       </c>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" spans="1:10" ht="93.6" customHeight="1">
+    <row r="20" spans="1:10" ht="93.5" customHeight="1">
       <c r="A20" s="13" t="s">
         <v>144</v>
       </c>
@@ -2197,7 +2203,7 @@
       </c>
       <c r="J20" s="13"/>
     </row>
-    <row r="21" spans="1:10" ht="197.45" customHeight="1">
+    <row r="21" spans="1:10" ht="197.5" customHeight="1">
       <c r="A21" s="13" t="s">
         <v>142</v>
       </c>
@@ -2221,11 +2227,11 @@
         <v>24</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" spans="1:10" ht="103.9" customHeight="1">
+    <row r="22" spans="1:10" ht="104" customHeight="1">
       <c r="A22" s="13" t="s">
         <v>33</v>
       </c>
@@ -2255,7 +2261,7 @@
       </c>
       <c r="J22" s="13"/>
     </row>
-    <row r="23" spans="1:10" ht="219.6" customHeight="1">
+    <row r="23" spans="1:10" ht="219.5" customHeight="1">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13" t="s">
@@ -2309,7 +2315,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="57">
+    <row r="25" spans="1:10" ht="80">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13" t="s">
@@ -2337,7 +2343,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="42.75">
+    <row r="26" spans="1:10" ht="48">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13" t="s">
@@ -2365,7 +2371,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="42.75">
+    <row r="27" spans="1:10" ht="64">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13" t="s">
@@ -2393,7 +2399,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="28.5">
+    <row r="28" spans="1:10" ht="48">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13" t="s">
@@ -2445,7 +2451,7 @@
       </c>
       <c r="J29" s="13"/>
     </row>
-    <row r="30" spans="1:10" ht="42.75">
+    <row r="30" spans="1:10" ht="64">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13" t="s">
@@ -2471,7 +2477,7 @@
       </c>
       <c r="J30" s="13"/>
     </row>
-    <row r="31" spans="1:10" ht="134.44999999999999" customHeight="1">
+    <row r="31" spans="1:10" ht="134.5" customHeight="1">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13" t="s">
@@ -2497,7 +2503,7 @@
       </c>
       <c r="J31" s="13"/>
     </row>
-    <row r="32" spans="1:10" ht="57">
+    <row r="32" spans="1:10" ht="96">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13" t="s">
@@ -2519,7 +2525,7 @@
         <v>24</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J32" s="13"/>
     </row>
@@ -2549,7 +2555,7 @@
       </c>
       <c r="J33" s="13"/>
     </row>
-    <row r="34" spans="1:10" ht="42.75">
+    <row r="34" spans="1:10" ht="48">
       <c r="A34" s="13" t="s">
         <v>33</v>
       </c>
@@ -2579,7 +2585,7 @@
       </c>
       <c r="J34" s="13"/>
     </row>
-    <row r="35" spans="1:10" ht="103.9" customHeight="1">
+    <row r="35" spans="1:10" ht="104" customHeight="1">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13" t="s">
@@ -2605,7 +2611,7 @@
       </c>
       <c r="J35" s="13"/>
     </row>
-    <row r="36" spans="1:10" ht="134.44999999999999" customHeight="1">
+    <row r="36" spans="1:10" ht="134.5" customHeight="1">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13" t="s">
@@ -2631,7 +2637,7 @@
       </c>
       <c r="J36" s="13"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" ht="32">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13" t="s">
@@ -2655,7 +2661,7 @@
       </c>
       <c r="J37" s="13"/>
     </row>
-    <row r="38" spans="1:10" ht="132.6" customHeight="1">
+    <row r="38" spans="1:10" ht="132.5" customHeight="1">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13" t="s">
@@ -2681,7 +2687,7 @@
       </c>
       <c r="J38" s="13"/>
     </row>
-    <row r="39" spans="1:10" ht="85.5">
+    <row r="39" spans="1:10" ht="112">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13" t="s">
@@ -2707,7 +2713,7 @@
       </c>
       <c r="J39" s="13"/>
     </row>
-    <row r="40" spans="1:10" ht="42.75">
+    <row r="40" spans="1:10" ht="48">
       <c r="A40" s="13" t="s">
         <v>165</v>
       </c>
@@ -2735,7 +2741,7 @@
       </c>
       <c r="J40" s="13"/>
     </row>
-    <row r="41" spans="1:10" ht="42.75">
+    <row r="41" spans="1:10" ht="64">
       <c r="A41" s="13" t="s">
         <v>33</v>
       </c>
@@ -2765,7 +2771,7 @@
       </c>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" ht="57">
+    <row r="42" spans="1:10" ht="64">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13" t="s">
@@ -2791,7 +2797,7 @@
       </c>
       <c r="J42" s="13"/>
     </row>
-    <row r="43" spans="1:10" ht="42.75">
+    <row r="43" spans="1:10" ht="48">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13" t="s">
@@ -2843,7 +2849,7 @@
       </c>
       <c r="J44" s="13"/>
     </row>
-    <row r="45" spans="1:10" ht="71.25">
+    <row r="45" spans="1:10" ht="96">
       <c r="A45" s="13" t="s">
         <v>33</v>
       </c>
@@ -2873,7 +2879,7 @@
       </c>
       <c r="J45" s="13"/>
     </row>
-    <row r="46" spans="1:10" ht="145.15" customHeight="1">
+    <row r="46" spans="1:10" ht="145.25" customHeight="1">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13" t="s">
@@ -2899,7 +2905,7 @@
       </c>
       <c r="J46" s="13"/>
     </row>
-    <row r="47" spans="1:10" ht="73.150000000000006" customHeight="1">
+    <row r="47" spans="1:10" ht="73.25" customHeight="1">
       <c r="A47" s="13" t="s">
         <v>110</v>
       </c>
@@ -2925,11 +2931,11 @@
         <v>24</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J47" s="13"/>
     </row>
-    <row r="48" spans="1:10" ht="156.75">
+    <row r="48" spans="1:10" ht="176">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13" t="s">
@@ -2955,7 +2961,7 @@
       </c>
       <c r="J48" s="13"/>
     </row>
-    <row r="49" spans="1:10" ht="128.25">
+    <row r="49" spans="1:10" ht="144">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13" t="s">
@@ -2981,7 +2987,7 @@
       </c>
       <c r="J49" s="13"/>
     </row>
-    <row r="50" spans="1:10" ht="78.599999999999994" customHeight="1">
+    <row r="50" spans="1:10" ht="78.5" customHeight="1">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13" t="s">
@@ -3002,12 +3008,12 @@
       <c r="H50" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I50" s="15" t="s">
-        <v>292</v>
+      <c r="I50" s="14" t="s">
+        <v>291</v>
       </c>
       <c r="J50" s="13"/>
     </row>
-    <row r="51" spans="1:10" ht="57">
+    <row r="51" spans="1:10" ht="64">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13" t="s">
@@ -3028,12 +3034,12 @@
       <c r="H51" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I51" s="15" t="s">
-        <v>292</v>
+      <c r="I51" s="14" t="s">
+        <v>291</v>
       </c>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" ht="71.25">
+    <row r="52" spans="1:10" ht="80">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13" t="s">
@@ -3054,12 +3060,12 @@
       <c r="H52" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I52" s="16" t="s">
-        <v>293</v>
+      <c r="I52" s="15" t="s">
+        <v>292</v>
       </c>
       <c r="J52" s="13"/>
     </row>
-    <row r="53" spans="1:10" ht="71.25">
+    <row r="53" spans="1:10" ht="80">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13" t="s">
@@ -3080,12 +3086,12 @@
       <c r="H53" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I53" s="16" t="s">
-        <v>293</v>
+      <c r="I53" s="15" t="s">
+        <v>292</v>
       </c>
       <c r="J53" s="13"/>
     </row>
-    <row r="54" spans="1:10" ht="30">
+    <row r="54" spans="1:10" ht="48">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13" t="s">
@@ -3106,8 +3112,8 @@
       <c r="H54" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I54" s="16" t="s">
-        <v>293</v>
+      <c r="I54" s="15" t="s">
+        <v>292</v>
       </c>
       <c r="J54" s="13"/>
     </row>
@@ -3163,7 +3169,7 @@
       </c>
       <c r="J56" s="13"/>
     </row>
-    <row r="57" spans="1:10" ht="83.45" customHeight="1">
+    <row r="57" spans="1:10" ht="83.5" customHeight="1">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13" t="s">
@@ -3189,7 +3195,7 @@
       </c>
       <c r="J57" s="13"/>
     </row>
-    <row r="58" spans="1:10" ht="156.75">
+    <row r="58" spans="1:10" ht="176">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13" t="s">
@@ -3215,7 +3221,7 @@
       </c>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" ht="156.75">
+    <row r="59" spans="1:10" ht="176">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13" t="s">
@@ -3241,7 +3247,7 @@
       </c>
       <c r="J59" s="13"/>
     </row>
-    <row r="60" spans="1:10" ht="99.75">
+    <row r="60" spans="1:10" ht="112">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13" t="s">
@@ -3267,7 +3273,7 @@
       </c>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" ht="128.25">
+    <row r="61" spans="1:10" ht="144">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13" t="s">
@@ -3293,7 +3299,7 @@
       </c>
       <c r="J61" s="13"/>
     </row>
-    <row r="62" spans="1:10" ht="71.25">
+    <row r="62" spans="1:10" ht="96">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13" t="s">
@@ -3319,7 +3325,7 @@
       </c>
       <c r="J62" s="13"/>
     </row>
-    <row r="63" spans="1:10" ht="28.5">
+    <row r="63" spans="1:10" ht="32">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13" t="s">
@@ -3346,17 +3352,17 @@
       <c r="J63" s="13"/>
     </row>
     <row r="68" spans="1:9" s="12" customFormat="1">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3408,11 +3414,11 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
@@ -3518,13 +3524,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" customWidth="1"/>
-    <col min="4" max="4" width="92.28515625" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" customWidth="1"/>
+    <col min="4" max="4" width="92.33203125" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
@@ -3541,7 +3547,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="40.9" customHeight="1">
+    <row r="3" spans="2:5" ht="41" customHeight="1">
       <c r="B3" s="4" t="s">
         <v>33</v>
       </c>
@@ -3553,7 +3559,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" ht="32">
       <c r="B4" s="4" t="s">
         <v>103</v>
       </c>
@@ -3565,7 +3571,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:5" ht="43.5">
+    <row r="5" spans="2:5" ht="48">
       <c r="B5" s="6" t="s">
         <v>110</v>
       </c>
@@ -3577,7 +3583,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" ht="16">
       <c r="B6" s="6" t="s">
         <v>142</v>
       </c>
@@ -3589,7 +3595,7 @@
       </c>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="2:5" ht="30">
+    <row r="7" spans="2:5" ht="32">
       <c r="B7" s="6" t="s">
         <v>144</v>
       </c>
@@ -3601,7 +3607,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" ht="16">
       <c r="B8" s="6" t="s">
         <v>165</v>
       </c>
@@ -3753,12 +3759,12 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="16">
       <c r="A1" s="7" t="s">
         <v>44</v>
       </c>
@@ -3774,7 +3780,7 @@
       <c r="D2" s="9"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="32">
       <c r="A3" s="6" t="s">
         <v>174</v>
       </c>
@@ -3790,7 +3796,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" ht="43.5">
+    <row r="5" spans="1:5" ht="64">
       <c r="A5" s="6" t="s">
         <v>176</v>
       </c>
@@ -3806,7 +3812,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:5" ht="29.25">
+    <row r="7" spans="1:5" ht="48">
       <c r="A7" s="6" t="s">
         <v>82</v>
       </c>
@@ -3822,7 +3828,7 @@
       <c r="D8" s="9"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="72">
+    <row r="9" spans="1:5" ht="112">
       <c r="A9" s="6" t="s">
         <v>175</v>
       </c>
@@ -3838,7 +3844,7 @@
       <c r="D10" s="9"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="72">
+    <row r="11" spans="1:5" ht="96">
       <c r="A11" s="6" t="s">
         <v>137</v>
       </c>
@@ -3854,7 +3860,7 @@
       <c r="D12" s="9"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="43.5">
+    <row r="13" spans="1:5" ht="64">
       <c r="A13" s="6" t="s">
         <v>150</v>
       </c>
@@ -3870,7 +3876,7 @@
       <c r="D14" s="9"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" ht="57.75">
+    <row r="15" spans="1:5" ht="80">
       <c r="A15" s="6" t="s">
         <v>154</v>
       </c>
@@ -3886,7 +3892,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="43.5">
+    <row r="17" spans="1:5" ht="48">
       <c r="A17" s="6" t="s">
         <v>170</v>
       </c>
@@ -3902,7 +3908,7 @@
       <c r="D18" s="9"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="29.25">
+    <row r="19" spans="1:5" ht="32">
       <c r="A19" s="6" t="s">
         <v>171</v>
       </c>
@@ -3916,7 +3922,7 @@
       <c r="C20" s="6"/>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:5" ht="43.5">
+    <row r="21" spans="1:5" ht="48">
       <c r="A21" s="6" t="s">
         <v>172</v>
       </c>
@@ -3930,7 +3936,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:5" ht="29.25">
+    <row r="23" spans="1:5" ht="32">
       <c r="A23" s="6" t="s">
         <v>177</v>
       </c>
@@ -3942,7 +3948,7 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="43.5">
+    <row r="25" spans="1:5" ht="64">
       <c r="A25" s="6" t="s">
         <v>178</v>
       </c>

</xml_diff>